<commit_message>
Ult act antes de presentar :100: hecho pa
Ya se generan las calificaciones y también los excel en la interfaz del profesor, también el alumnos ya puede verlos.
Terminado totalmente según la carpeta del proyecto
</commit_message>
<xml_diff>
--- a/media/Planilla de Proceso.xlsx
+++ b/media/Planilla de Proceso.xlsx
@@ -547,7 +547,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -887,11 +887,20 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="27" fillId="5" borderId="9" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="164" fontId="27" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
@@ -925,6 +934,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -1452,7 +1467,7 @@
       </c>
       <c r="B5" s="121" t="n"/>
       <c r="C5" s="73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
@@ -1540,18 +1555,22 @@
       <c r="D6" s="123" t="n"/>
       <c r="E6" s="123" t="n"/>
       <c r="F6" s="124" t="n"/>
-      <c r="G6" s="74" t="n"/>
-      <c r="H6" s="74" t="n"/>
-      <c r="I6" s="74" t="n"/>
-      <c r="J6" s="74" t="n"/>
-      <c r="K6" s="74" t="n"/>
-      <c r="L6" s="74" t="n"/>
-      <c r="M6" s="74" t="n"/>
-      <c r="N6" s="74" t="n"/>
-      <c r="O6" s="74" t="n"/>
-      <c r="P6" s="74" t="n"/>
-      <c r="Q6" s="74" t="n"/>
-      <c r="R6" s="74" t="n"/>
+      <c r="G6" s="74" t="n">
+        <v>44918</v>
+      </c>
+      <c r="H6" s="123" t="n"/>
+      <c r="I6" s="123" t="n"/>
+      <c r="J6" s="123" t="n"/>
+      <c r="K6" s="123" t="n"/>
+      <c r="L6" s="124" t="n"/>
+      <c r="M6" s="74" t="n">
+        <v>44918</v>
+      </c>
+      <c r="N6" s="123" t="n"/>
+      <c r="O6" s="123" t="n"/>
+      <c r="P6" s="123" t="n"/>
+      <c r="Q6" s="123" t="n"/>
+      <c r="R6" s="124" t="n"/>
       <c r="S6" s="74" t="n"/>
       <c r="T6" s="74" t="n"/>
       <c r="U6" s="74" t="n"/>
@@ -1621,17 +1640,17 @@
       <c r="E7" s="123" t="n"/>
       <c r="F7" s="124" t="n"/>
       <c r="G7" s="75" t="n"/>
-      <c r="H7" s="75" t="n"/>
-      <c r="I7" s="75" t="n"/>
-      <c r="J7" s="75" t="n"/>
-      <c r="K7" s="75" t="n"/>
-      <c r="L7" s="75" t="n"/>
+      <c r="H7" s="123" t="n"/>
+      <c r="I7" s="123" t="n"/>
+      <c r="J7" s="123" t="n"/>
+      <c r="K7" s="123" t="n"/>
+      <c r="L7" s="124" t="n"/>
       <c r="M7" s="75" t="n"/>
-      <c r="N7" s="75" t="n"/>
-      <c r="O7" s="75" t="n"/>
-      <c r="P7" s="75" t="n"/>
-      <c r="Q7" s="75" t="n"/>
-      <c r="R7" s="75" t="n"/>
+      <c r="N7" s="123" t="n"/>
+      <c r="O7" s="123" t="n"/>
+      <c r="P7" s="123" t="n"/>
+      <c r="Q7" s="123" t="n"/>
+      <c r="R7" s="124" t="n"/>
       <c r="S7" s="75" t="n"/>
       <c r="T7" s="75" t="n"/>
       <c r="U7" s="75" t="n"/>
@@ -1697,17 +1716,17 @@
       <c r="E8" s="123" t="n"/>
       <c r="F8" s="124" t="n"/>
       <c r="G8" s="76" t="n"/>
-      <c r="H8" s="76" t="n"/>
-      <c r="I8" s="76" t="n"/>
-      <c r="J8" s="76" t="n"/>
-      <c r="K8" s="76" t="n"/>
-      <c r="L8" s="76" t="n"/>
+      <c r="H8" s="123" t="n"/>
+      <c r="I8" s="123" t="n"/>
+      <c r="J8" s="123" t="n"/>
+      <c r="K8" s="123" t="n"/>
+      <c r="L8" s="124" t="n"/>
       <c r="M8" s="76" t="n"/>
-      <c r="N8" s="76" t="n"/>
-      <c r="O8" s="76" t="n"/>
-      <c r="P8" s="76" t="n"/>
-      <c r="Q8" s="76" t="n"/>
-      <c r="R8" s="76" t="n"/>
+      <c r="N8" s="123" t="n"/>
+      <c r="O8" s="123" t="n"/>
+      <c r="P8" s="123" t="n"/>
+      <c r="Q8" s="123" t="n"/>
+      <c r="R8" s="124" t="n"/>
       <c r="S8" s="76" t="n"/>
       <c r="T8" s="76" t="n"/>
       <c r="U8" s="76" t="n"/>
@@ -1770,24 +1789,32 @@
       <c r="B9" s="122" t="n"/>
       <c r="C9" s="76" t="inlineStr">
         <is>
-          <t>Quimicos Historicos</t>
+          <t>Animales</t>
         </is>
       </c>
       <c r="D9" s="123" t="n"/>
       <c r="E9" s="123" t="n"/>
       <c r="F9" s="124" t="n"/>
-      <c r="G9" s="76" t="n"/>
-      <c r="H9" s="76" t="n"/>
-      <c r="I9" s="76" t="n"/>
-      <c r="J9" s="76" t="n"/>
-      <c r="K9" s="76" t="n"/>
-      <c r="L9" s="76" t="n"/>
-      <c r="M9" s="76" t="n"/>
-      <c r="N9" s="76" t="n"/>
-      <c r="O9" s="76" t="n"/>
-      <c r="P9" s="76" t="n"/>
-      <c r="Q9" s="76" t="n"/>
-      <c r="R9" s="76" t="n"/>
+      <c r="G9" s="76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Metamorfosis </t>
+        </is>
+      </c>
+      <c r="H9" s="123" t="n"/>
+      <c r="I9" s="123" t="n"/>
+      <c r="J9" s="123" t="n"/>
+      <c r="K9" s="123" t="n"/>
+      <c r="L9" s="124" t="n"/>
+      <c r="M9" s="76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Célula </t>
+        </is>
+      </c>
+      <c r="N9" s="123" t="n"/>
+      <c r="O9" s="123" t="n"/>
+      <c r="P9" s="123" t="n"/>
+      <c r="Q9" s="123" t="n"/>
+      <c r="R9" s="124" t="n"/>
       <c r="S9" s="76" t="n"/>
       <c r="T9" s="76" t="n"/>
       <c r="U9" s="76" t="n"/>
@@ -1853,17 +1880,17 @@
       <c r="E10" s="123" t="n"/>
       <c r="F10" s="124" t="n"/>
       <c r="G10" s="76" t="n"/>
-      <c r="H10" s="76" t="n"/>
-      <c r="I10" s="76" t="n"/>
-      <c r="J10" s="76" t="n"/>
-      <c r="K10" s="76" t="n"/>
-      <c r="L10" s="76" t="n"/>
+      <c r="H10" s="123" t="n"/>
+      <c r="I10" s="123" t="n"/>
+      <c r="J10" s="123" t="n"/>
+      <c r="K10" s="123" t="n"/>
+      <c r="L10" s="124" t="n"/>
       <c r="M10" s="76" t="n"/>
-      <c r="N10" s="76" t="n"/>
-      <c r="O10" s="76" t="n"/>
-      <c r="P10" s="76" t="n"/>
-      <c r="Q10" s="76" t="n"/>
-      <c r="R10" s="76" t="n"/>
+      <c r="N10" s="123" t="n"/>
+      <c r="O10" s="123" t="n"/>
+      <c r="P10" s="123" t="n"/>
+      <c r="Q10" s="123" t="n"/>
+      <c r="R10" s="124" t="n"/>
       <c r="S10" s="76" t="n"/>
       <c r="T10" s="76" t="n"/>
       <c r="U10" s="76" t="n"/>
@@ -1931,12 +1958,12 @@
       </c>
       <c r="D11" s="68" t="inlineStr">
         <is>
-          <t>Esucha tus compas</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E11" s="68" t="inlineStr">
         <is>
-          <t>Perseverancia y xd</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F11" s="134" t="inlineStr">
@@ -1944,18 +1971,66 @@
           <t>TOTAL INDICADORES LOGRADOS</t>
         </is>
       </c>
-      <c r="G11" s="69" t="n"/>
-      <c r="H11" s="67" t="n"/>
-      <c r="I11" s="67" t="n"/>
-      <c r="J11" s="67" t="n"/>
-      <c r="K11" s="67" t="n"/>
-      <c r="L11" s="69" t="n"/>
-      <c r="M11" s="68" t="n"/>
-      <c r="N11" s="68" t="n"/>
-      <c r="O11" s="68" t="n"/>
-      <c r="P11" s="68" t="n"/>
-      <c r="Q11" s="69" t="n"/>
-      <c r="R11" s="70" t="n"/>
+      <c r="G11" s="69" t="inlineStr">
+        <is>
+          <t>Entrega en Fecha</t>
+        </is>
+      </c>
+      <c r="H11" s="67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cumple los requisitos </t>
+        </is>
+      </c>
+      <c r="I11" s="67" t="inlineStr">
+        <is>
+          <t>Identifica todo los identifica</t>
+        </is>
+      </c>
+      <c r="J11" s="67" t="inlineStr">
+        <is>
+          <t>Creatividad</t>
+        </is>
+      </c>
+      <c r="K11" s="67" t="inlineStr">
+        <is>
+          <t>Otro indicador</t>
+        </is>
+      </c>
+      <c r="L11" s="135" t="inlineStr">
+        <is>
+          <t>TOTAL INDICADORES LOGRADOS</t>
+        </is>
+      </c>
+      <c r="M11" s="68" t="inlineStr">
+        <is>
+          <t>Entrega en Fecha</t>
+        </is>
+      </c>
+      <c r="N11" s="68" t="inlineStr">
+        <is>
+          <t>Esucha tus compas</t>
+        </is>
+      </c>
+      <c r="O11" s="68" t="inlineStr">
+        <is>
+          <t>Completa totalmente</t>
+        </is>
+      </c>
+      <c r="P11" s="68" t="inlineStr">
+        <is>
+          <t>Pulcritud</t>
+        </is>
+      </c>
+      <c r="Q11" s="69" t="inlineStr">
+        <is>
+          <t>Creatividad</t>
+        </is>
+      </c>
+      <c r="R11" s="136" t="inlineStr">
+        <is>
+          <t>TOTAL INDICADORES LOGRADOS</t>
+        </is>
+      </c>
       <c r="S11" s="70" t="n"/>
       <c r="T11" s="70" t="n"/>
       <c r="U11" s="70" t="n"/>
@@ -2032,26 +2107,50 @@
         <v>2</v>
       </c>
       <c r="D12" s="82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="82" t="n">
         <v>2</v>
       </c>
-      <c r="F12" s="135" t="n">
-        <v>6</v>
-      </c>
-      <c r="G12" s="82" t="n"/>
-      <c r="H12" s="82" t="n"/>
-      <c r="I12" s="82" t="n"/>
-      <c r="J12" s="82" t="n"/>
-      <c r="K12" s="82" t="n"/>
-      <c r="L12" s="82" t="n"/>
-      <c r="M12" s="82" t="n"/>
-      <c r="N12" s="82" t="n"/>
-      <c r="O12" s="82" t="n"/>
-      <c r="P12" s="82" t="n"/>
-      <c r="Q12" s="82" t="n"/>
-      <c r="R12" s="82" t="n"/>
+      <c r="F12" s="137" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" s="137" t="n">
+        <v>10</v>
+      </c>
+      <c r="M12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="82" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" s="137" t="n">
+        <v>10</v>
+      </c>
       <c r="S12" s="82" t="n"/>
       <c r="T12" s="82" t="n"/>
       <c r="U12" s="82" t="n"/>
@@ -2124,26 +2223,50 @@
         <v>2</v>
       </c>
       <c r="D13" s="83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="83" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="136" t="n">
-        <v>6</v>
-      </c>
-      <c r="G13" s="84" t="n"/>
-      <c r="H13" s="83" t="n"/>
-      <c r="I13" s="83" t="n"/>
-      <c r="J13" s="83" t="n"/>
-      <c r="K13" s="83" t="n"/>
-      <c r="L13" s="84" t="n"/>
-      <c r="M13" s="83" t="n"/>
-      <c r="N13" s="83" t="n"/>
-      <c r="O13" s="83" t="n"/>
-      <c r="P13" s="83" t="n"/>
-      <c r="Q13" s="84" t="n"/>
-      <c r="R13" s="83" t="n"/>
+      <c r="F13" s="138" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" s="84" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" s="139" t="n">
+        <v>8</v>
+      </c>
+      <c r="M13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="N13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="84" t="n">
+        <v>2</v>
+      </c>
+      <c r="R13" s="138" t="n">
+        <v>10</v>
+      </c>
       <c r="S13" s="83" t="n"/>
       <c r="T13" s="83" t="n"/>
       <c r="U13" s="83" t="n"/>
@@ -2200,7 +2323,7 @@
         <v/>
       </c>
       <c r="BP13" s="29" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="BQ13" s="60" t="n"/>
       <c r="BR13" s="60" t="n"/>
@@ -2218,26 +2341,50 @@
         <v>2</v>
       </c>
       <c r="D14" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="138" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="83" t="n">
+      <c r="H14" s="83" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="136" t="n">
-        <v>6</v>
-      </c>
-      <c r="G14" s="84" t="n"/>
-      <c r="H14" s="83" t="n"/>
-      <c r="I14" s="83" t="n"/>
-      <c r="J14" s="83" t="n"/>
-      <c r="K14" s="83" t="n"/>
-      <c r="L14" s="84" t="n"/>
-      <c r="M14" s="83" t="n"/>
-      <c r="N14" s="83" t="n"/>
-      <c r="O14" s="83" t="n"/>
-      <c r="P14" s="83" t="n"/>
-      <c r="Q14" s="84" t="n"/>
-      <c r="R14" s="83" t="n"/>
+      <c r="I14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="139" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="138" t="n">
+        <v>2</v>
+      </c>
       <c r="S14" s="83" t="n"/>
       <c r="T14" s="83" t="n"/>
       <c r="U14" s="83" t="n"/>
@@ -2294,7 +2441,7 @@
         <v/>
       </c>
       <c r="BP14" s="29" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BQ14" s="60" t="n"/>
       <c r="BR14" s="60" t="n"/>
@@ -2312,26 +2459,50 @@
         <v>2</v>
       </c>
       <c r="D15" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="138" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="83" t="n">
+      <c r="G15" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="F15" s="136" t="n">
+      <c r="H15" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="L15" s="139" t="n">
+        <v>10</v>
+      </c>
+      <c r="M15" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="N15" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="84" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" s="138" t="n">
         <v>6</v>
       </c>
-      <c r="G15" s="84" t="n"/>
-      <c r="H15" s="83" t="n"/>
-      <c r="I15" s="83" t="n"/>
-      <c r="J15" s="83" t="n"/>
-      <c r="K15" s="83" t="n"/>
-      <c r="L15" s="84" t="n"/>
-      <c r="M15" s="83" t="n"/>
-      <c r="N15" s="83" t="n"/>
-      <c r="O15" s="83" t="n"/>
-      <c r="P15" s="83" t="n"/>
-      <c r="Q15" s="84" t="n"/>
-      <c r="R15" s="83" t="n"/>
       <c r="S15" s="83" t="n"/>
       <c r="T15" s="83" t="n"/>
       <c r="U15" s="83" t="n"/>
@@ -2388,7 +2559,7 @@
         <v/>
       </c>
       <c r="BP15" s="29" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="BQ15" s="60" t="n"/>
       <c r="BR15" s="60" t="n"/>
@@ -3755,7 +3926,7 @@
     </row>
     <row r="33" ht="21" customHeight="1">
       <c r="A33" s="38" t="n"/>
-      <c r="B33" s="137" t="n"/>
+      <c r="B33" s="140" t="n"/>
       <c r="C33" s="79" t="n"/>
       <c r="D33" s="79" t="n"/>
       <c r="E33" s="79" t="n"/>
@@ -3827,7 +3998,7 @@
     </row>
     <row r="34" ht="21" customHeight="1">
       <c r="A34" s="43" t="n"/>
-      <c r="B34" s="138" t="n"/>
+      <c r="B34" s="141" t="n"/>
       <c r="C34" s="79" t="n"/>
       <c r="D34" s="79" t="n"/>
       <c r="E34" s="79" t="n"/>
@@ -3899,7 +4070,7 @@
     </row>
     <row r="35" ht="21" customHeight="1">
       <c r="A35" s="43" t="n"/>
-      <c r="B35" s="138" t="n"/>
+      <c r="B35" s="141" t="n"/>
       <c r="C35" s="79" t="n"/>
       <c r="D35" s="79" t="n"/>
       <c r="E35" s="79" t="n"/>
@@ -3976,17 +4147,17 @@
         </is>
       </c>
       <c r="B36" s="126" t="n"/>
-      <c r="C36" s="139" t="n"/>
+      <c r="C36" s="142" t="n"/>
       <c r="D36" s="122" t="n"/>
       <c r="E36" s="122" t="n"/>
       <c r="F36" s="122" t="n"/>
       <c r="G36" s="126" t="n"/>
-      <c r="H36" s="139" t="n"/>
+      <c r="H36" s="142" t="n"/>
       <c r="I36" s="122" t="n"/>
       <c r="J36" s="122" t="n"/>
       <c r="K36" s="122" t="n"/>
       <c r="L36" s="126" t="n"/>
-      <c r="M36" s="139" t="n"/>
+      <c r="M36" s="142" t="n"/>
       <c r="N36" s="122" t="n"/>
       <c r="O36" s="122" t="n"/>
       <c r="P36" s="122" t="n"/>
@@ -4001,17 +4172,17 @@
       <c r="Y36" s="122" t="n"/>
       <c r="Z36" s="122" t="n"/>
       <c r="AA36" s="126" t="n"/>
-      <c r="AB36" s="139" t="n"/>
+      <c r="AB36" s="142" t="n"/>
       <c r="AC36" s="122" t="n"/>
       <c r="AD36" s="122" t="n"/>
       <c r="AE36" s="122" t="n"/>
       <c r="AF36" s="126" t="n"/>
-      <c r="AG36" s="139" t="n"/>
+      <c r="AG36" s="142" t="n"/>
       <c r="AH36" s="122" t="n"/>
       <c r="AI36" s="122" t="n"/>
       <c r="AJ36" s="122" t="n"/>
       <c r="AK36" s="126" t="n"/>
-      <c r="AL36" s="139" t="n"/>
+      <c r="AL36" s="142" t="n"/>
       <c r="AM36" s="122" t="n"/>
       <c r="AN36" s="122" t="n"/>
       <c r="AO36" s="122" t="n"/>
@@ -4021,12 +4192,12 @@
       <c r="AS36" s="122" t="n"/>
       <c r="AT36" s="122" t="n"/>
       <c r="AU36" s="126" t="n"/>
-      <c r="AV36" s="139" t="n"/>
+      <c r="AV36" s="142" t="n"/>
       <c r="AW36" s="122" t="n"/>
       <c r="AX36" s="122" t="n"/>
       <c r="AY36" s="122" t="n"/>
       <c r="AZ36" s="126" t="n"/>
-      <c r="BA36" s="139" t="n"/>
+      <c r="BA36" s="142" t="n"/>
       <c r="BB36" s="122" t="n"/>
       <c r="BC36" s="122" t="n"/>
       <c r="BD36" s="122" t="n"/>
@@ -4050,68 +4221,68 @@
       <c r="BR36" s="60" t="n"/>
     </row>
     <row r="37" ht="79.5" customHeight="1">
-      <c r="A37" s="140" t="inlineStr">
+      <c r="A37" s="143" t="inlineStr">
         <is>
           <t xml:space="preserve"> CAPACIDADES ===&gt;&gt;</t>
         </is>
       </c>
       <c r="B37" s="126" t="n"/>
-      <c r="C37" s="141" t="n"/>
+      <c r="C37" s="144" t="n"/>
       <c r="D37" s="122" t="n"/>
       <c r="E37" s="122" t="n"/>
       <c r="F37" s="122" t="n"/>
       <c r="G37" s="126" t="n"/>
-      <c r="H37" s="142" t="n"/>
+      <c r="H37" s="145" t="n"/>
       <c r="I37" s="122" t="n"/>
       <c r="J37" s="122" t="n"/>
       <c r="K37" s="122" t="n"/>
       <c r="L37" s="126" t="n"/>
-      <c r="M37" s="142" t="n"/>
+      <c r="M37" s="145" t="n"/>
       <c r="N37" s="122" t="n"/>
       <c r="O37" s="122" t="n"/>
       <c r="P37" s="122" t="n"/>
       <c r="Q37" s="126" t="n"/>
-      <c r="R37" s="143" t="n"/>
+      <c r="R37" s="146" t="n"/>
       <c r="S37" s="122" t="n"/>
       <c r="T37" s="122" t="n"/>
       <c r="U37" s="122" t="n"/>
       <c r="V37" s="126" t="n"/>
-      <c r="W37" s="144" t="n"/>
+      <c r="W37" s="147" t="n"/>
       <c r="X37" s="122" t="n"/>
       <c r="Y37" s="122" t="n"/>
       <c r="Z37" s="122" t="n"/>
       <c r="AA37" s="126" t="n"/>
-      <c r="AB37" s="145" t="n"/>
+      <c r="AB37" s="148" t="n"/>
       <c r="AC37" s="122" t="n"/>
       <c r="AD37" s="122" t="n"/>
       <c r="AE37" s="122" t="n"/>
       <c r="AF37" s="126" t="n"/>
-      <c r="AG37" s="145" t="n"/>
+      <c r="AG37" s="148" t="n"/>
       <c r="AH37" s="122" t="n"/>
       <c r="AI37" s="122" t="n"/>
       <c r="AJ37" s="122" t="n"/>
       <c r="AK37" s="126" t="n"/>
-      <c r="AL37" s="145" t="n"/>
+      <c r="AL37" s="148" t="n"/>
       <c r="AM37" s="122" t="n"/>
       <c r="AN37" s="122" t="n"/>
       <c r="AO37" s="122" t="n"/>
       <c r="AP37" s="126" t="n"/>
-      <c r="AQ37" s="144" t="n"/>
+      <c r="AQ37" s="147" t="n"/>
       <c r="AR37" s="122" t="n"/>
       <c r="AS37" s="122" t="n"/>
       <c r="AT37" s="122" t="n"/>
       <c r="AU37" s="126" t="n"/>
-      <c r="AV37" s="145" t="n"/>
+      <c r="AV37" s="148" t="n"/>
       <c r="AW37" s="122" t="n"/>
       <c r="AX37" s="122" t="n"/>
       <c r="AY37" s="122" t="n"/>
       <c r="AZ37" s="126" t="n"/>
-      <c r="BA37" s="145" t="n"/>
+      <c r="BA37" s="148" t="n"/>
       <c r="BB37" s="122" t="n"/>
       <c r="BC37" s="122" t="n"/>
       <c r="BD37" s="122" t="n"/>
       <c r="BE37" s="126" t="n"/>
-      <c r="BF37" s="146" t="n"/>
+      <c r="BF37" s="149" t="n"/>
       <c r="BG37" s="122" t="n"/>
       <c r="BH37" s="122" t="n"/>
       <c r="BI37" s="122" t="n"/>
@@ -4208,21 +4379,21 @@
         </is>
       </c>
       <c r="B39" s="126" t="n"/>
-      <c r="C39" s="147" t="n"/>
-      <c r="D39" s="148" t="n"/>
-      <c r="E39" s="148" t="n"/>
-      <c r="F39" s="148" t="n"/>
-      <c r="G39" s="149" t="n"/>
-      <c r="H39" s="147" t="n"/>
-      <c r="I39" s="148" t="n"/>
-      <c r="J39" s="148" t="n"/>
-      <c r="K39" s="148" t="n"/>
-      <c r="L39" s="149" t="n"/>
-      <c r="M39" s="147" t="n"/>
-      <c r="N39" s="148" t="n"/>
-      <c r="O39" s="148" t="n"/>
-      <c r="P39" s="148" t="n"/>
-      <c r="Q39" s="149" t="n"/>
+      <c r="C39" s="150" t="n"/>
+      <c r="D39" s="151" t="n"/>
+      <c r="E39" s="151" t="n"/>
+      <c r="F39" s="151" t="n"/>
+      <c r="G39" s="152" t="n"/>
+      <c r="H39" s="150" t="n"/>
+      <c r="I39" s="151" t="n"/>
+      <c r="J39" s="151" t="n"/>
+      <c r="K39" s="151" t="n"/>
+      <c r="L39" s="152" t="n"/>
+      <c r="M39" s="150" t="n"/>
+      <c r="N39" s="151" t="n"/>
+      <c r="O39" s="151" t="n"/>
+      <c r="P39" s="151" t="n"/>
+      <c r="Q39" s="152" t="n"/>
       <c r="R39" s="117" t="n"/>
       <c r="S39" s="13" t="n"/>
       <c r="T39" s="13" t="n"/>
@@ -4233,36 +4404,36 @@
       <c r="Y39" s="13" t="n"/>
       <c r="Z39" s="13" t="n"/>
       <c r="AA39" s="14" t="n"/>
-      <c r="AB39" s="147" t="n"/>
-      <c r="AC39" s="148" t="n"/>
-      <c r="AD39" s="148" t="n"/>
-      <c r="AE39" s="148" t="n"/>
-      <c r="AF39" s="149" t="n"/>
-      <c r="AG39" s="147" t="n"/>
-      <c r="AH39" s="148" t="n"/>
-      <c r="AI39" s="148" t="n"/>
-      <c r="AJ39" s="148" t="n"/>
-      <c r="AK39" s="149" t="n"/>
-      <c r="AL39" s="147" t="n"/>
-      <c r="AM39" s="148" t="n"/>
-      <c r="AN39" s="148" t="n"/>
-      <c r="AO39" s="148" t="n"/>
-      <c r="AP39" s="149" t="n"/>
+      <c r="AB39" s="150" t="n"/>
+      <c r="AC39" s="151" t="n"/>
+      <c r="AD39" s="151" t="n"/>
+      <c r="AE39" s="151" t="n"/>
+      <c r="AF39" s="152" t="n"/>
+      <c r="AG39" s="150" t="n"/>
+      <c r="AH39" s="151" t="n"/>
+      <c r="AI39" s="151" t="n"/>
+      <c r="AJ39" s="151" t="n"/>
+      <c r="AK39" s="152" t="n"/>
+      <c r="AL39" s="150" t="n"/>
+      <c r="AM39" s="151" t="n"/>
+      <c r="AN39" s="151" t="n"/>
+      <c r="AO39" s="151" t="n"/>
+      <c r="AP39" s="152" t="n"/>
       <c r="AQ39" s="117" t="n"/>
       <c r="AR39" s="13" t="n"/>
       <c r="AS39" s="13" t="n"/>
       <c r="AT39" s="13" t="n"/>
       <c r="AU39" s="14" t="n"/>
-      <c r="AV39" s="147" t="n"/>
-      <c r="AW39" s="148" t="n"/>
-      <c r="AX39" s="148" t="n"/>
-      <c r="AY39" s="148" t="n"/>
-      <c r="AZ39" s="149" t="n"/>
-      <c r="BA39" s="147" t="n"/>
-      <c r="BB39" s="148" t="n"/>
-      <c r="BC39" s="148" t="n"/>
-      <c r="BD39" s="148" t="n"/>
-      <c r="BE39" s="149" t="n"/>
+      <c r="AV39" s="150" t="n"/>
+      <c r="AW39" s="151" t="n"/>
+      <c r="AX39" s="151" t="n"/>
+      <c r="AY39" s="151" t="n"/>
+      <c r="AZ39" s="152" t="n"/>
+      <c r="BA39" s="150" t="n"/>
+      <c r="BB39" s="151" t="n"/>
+      <c r="BC39" s="151" t="n"/>
+      <c r="BD39" s="151" t="n"/>
+      <c r="BE39" s="152" t="n"/>
       <c r="BF39" s="117" t="n"/>
       <c r="BG39" s="13" t="n"/>
       <c r="BH39" s="13" t="n"/>
@@ -4367,31 +4538,79 @@
       </c>
       <c r="D41" s="65" t="inlineStr">
         <is>
-          <t>Esucha tus compas</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E41" s="65" t="inlineStr">
         <is>
-          <t>Perseverancia y xd</t>
+          <t>B</t>
         </is>
       </c>
-      <c r="F41" s="150" t="inlineStr">
+      <c r="F41" s="153" t="inlineStr">
         <is>
           <t>TOTAL INDICADORES LOGRADOS</t>
         </is>
       </c>
-      <c r="G41" s="71" t="n"/>
-      <c r="H41" s="64" t="n"/>
-      <c r="I41" s="64" t="n"/>
-      <c r="J41" s="64" t="n"/>
-      <c r="K41" s="64" t="n"/>
-      <c r="L41" s="71" t="n"/>
-      <c r="M41" s="65" t="n"/>
-      <c r="N41" s="65" t="n"/>
-      <c r="O41" s="65" t="n"/>
-      <c r="P41" s="65" t="n"/>
-      <c r="Q41" s="71" t="n"/>
-      <c r="R41" s="72" t="n"/>
+      <c r="G41" s="71" t="inlineStr">
+        <is>
+          <t>Entrega en Fecha</t>
+        </is>
+      </c>
+      <c r="H41" s="64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cumple los requisitos </t>
+        </is>
+      </c>
+      <c r="I41" s="64" t="inlineStr">
+        <is>
+          <t>Identifica todo los identifica</t>
+        </is>
+      </c>
+      <c r="J41" s="64" t="inlineStr">
+        <is>
+          <t>Creatividad</t>
+        </is>
+      </c>
+      <c r="K41" s="64" t="inlineStr">
+        <is>
+          <t>Otro indicador</t>
+        </is>
+      </c>
+      <c r="L41" s="154" t="inlineStr">
+        <is>
+          <t>TOTAL INDICADORES LOGRADOS</t>
+        </is>
+      </c>
+      <c r="M41" s="65" t="inlineStr">
+        <is>
+          <t>Entrega en Fecha</t>
+        </is>
+      </c>
+      <c r="N41" s="65" t="inlineStr">
+        <is>
+          <t>Esucha tus compas</t>
+        </is>
+      </c>
+      <c r="O41" s="65" t="inlineStr">
+        <is>
+          <t>Completa totalmente</t>
+        </is>
+      </c>
+      <c r="P41" s="65" t="inlineStr">
+        <is>
+          <t>Pulcritud</t>
+        </is>
+      </c>
+      <c r="Q41" s="71" t="inlineStr">
+        <is>
+          <t>Creatividad</t>
+        </is>
+      </c>
+      <c r="R41" s="155" t="inlineStr">
+        <is>
+          <t>TOTAL INDICADORES LOGRADOS</t>
+        </is>
+      </c>
       <c r="S41" s="72" t="n"/>
       <c r="T41" s="72" t="n"/>
       <c r="U41" s="72" t="n"/>
@@ -4468,26 +4687,50 @@
         <v>2</v>
       </c>
       <c r="D42" s="85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="F42" s="151" t="n">
-        <v>6</v>
-      </c>
-      <c r="G42" s="85" t="n"/>
-      <c r="H42" s="85" t="n"/>
-      <c r="I42" s="85" t="n"/>
-      <c r="J42" s="85" t="n"/>
-      <c r="K42" s="85" t="n"/>
-      <c r="L42" s="85" t="n"/>
-      <c r="M42" s="85" t="n"/>
-      <c r="N42" s="85" t="n"/>
-      <c r="O42" s="85" t="n"/>
-      <c r="P42" s="85" t="n"/>
-      <c r="Q42" s="85" t="n"/>
-      <c r="R42" s="85" t="n"/>
+      <c r="F42" s="156" t="n">
+        <v>5</v>
+      </c>
+      <c r="G42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="H42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="I42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="J42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="K42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="L42" s="156" t="n">
+        <v>10</v>
+      </c>
+      <c r="M42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="N42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="O42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="P42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="R42" s="156" t="n">
+        <v>10</v>
+      </c>
       <c r="S42" s="85" t="n"/>
       <c r="T42" s="85" t="n"/>
       <c r="U42" s="85" t="n"/>
@@ -4551,7 +4794,7 @@
       <c r="A43" s="26" t="n">
         <v>21</v>
       </c>
-      <c r="B43" s="152" t="n"/>
+      <c r="B43" s="157" t="n"/>
       <c r="C43" s="86" t="n"/>
       <c r="D43" s="86" t="n"/>
       <c r="E43" s="86" t="n"/>
@@ -4631,7 +4874,7 @@
       <c r="A44" s="26" t="n">
         <v>22</v>
       </c>
-      <c r="B44" s="153" t="n"/>
+      <c r="B44" s="158" t="n"/>
       <c r="C44" s="86" t="n"/>
       <c r="D44" s="86" t="n"/>
       <c r="E44" s="86" t="n"/>
@@ -4711,7 +4954,7 @@
       <c r="A45" s="26" t="n">
         <v>23</v>
       </c>
-      <c r="B45" s="153" t="n"/>
+      <c r="B45" s="158" t="n"/>
       <c r="C45" s="86" t="n"/>
       <c r="D45" s="86" t="n"/>
       <c r="E45" s="86" t="n"/>
@@ -4791,7 +5034,7 @@
       <c r="A46" s="26" t="n">
         <v>24</v>
       </c>
-      <c r="B46" s="154" t="n"/>
+      <c r="B46" s="159" t="n"/>
       <c r="C46" s="86" t="n"/>
       <c r="D46" s="86" t="n"/>
       <c r="E46" s="86" t="n"/>
@@ -4871,7 +5114,7 @@
       <c r="A47" s="26" t="n">
         <v>25</v>
       </c>
-      <c r="B47" s="155" t="n"/>
+      <c r="B47" s="160" t="n"/>
       <c r="C47" s="86" t="n"/>
       <c r="D47" s="86" t="n"/>
       <c r="E47" s="86" t="n"/>
@@ -4951,7 +5194,7 @@
       <c r="A48" s="26" t="n">
         <v>26</v>
       </c>
-      <c r="B48" s="156" t="n"/>
+      <c r="B48" s="161" t="n"/>
       <c r="C48" s="86" t="n"/>
       <c r="D48" s="86" t="n"/>
       <c r="E48" s="86" t="n"/>
@@ -5031,7 +5274,7 @@
       <c r="A49" s="26" t="n">
         <v>27</v>
       </c>
-      <c r="B49" s="156" t="n"/>
+      <c r="B49" s="161" t="n"/>
       <c r="C49" s="86" t="n"/>
       <c r="D49" s="86" t="n"/>
       <c r="E49" s="86" t="n"/>
@@ -5111,7 +5354,7 @@
       <c r="A50" s="26" t="n">
         <v>28</v>
       </c>
-      <c r="B50" s="157" t="n"/>
+      <c r="B50" s="162" t="n"/>
       <c r="C50" s="86" t="n"/>
       <c r="D50" s="86" t="n"/>
       <c r="E50" s="86" t="n"/>
@@ -5191,7 +5434,7 @@
       <c r="A51" s="26" t="n">
         <v>29</v>
       </c>
-      <c r="B51" s="156" t="n"/>
+      <c r="B51" s="161" t="n"/>
       <c r="C51" s="86" t="n"/>
       <c r="D51" s="86" t="n"/>
       <c r="E51" s="86" t="n"/>
@@ -5271,7 +5514,7 @@
       <c r="A52" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="B52" s="156" t="n"/>
+      <c r="B52" s="161" t="n"/>
       <c r="C52" s="86" t="n"/>
       <c r="D52" s="86" t="n"/>
       <c r="E52" s="86" t="n"/>
@@ -5351,7 +5594,7 @@
       <c r="A53" s="26" t="n">
         <v>31</v>
       </c>
-      <c r="B53" s="156" t="n"/>
+      <c r="B53" s="161" t="n"/>
       <c r="C53" s="86" t="n"/>
       <c r="D53" s="86" t="n"/>
       <c r="E53" s="86" t="n"/>
@@ -5431,7 +5674,7 @@
       <c r="A54" s="26" t="n">
         <v>32</v>
       </c>
-      <c r="B54" s="158" t="n"/>
+      <c r="B54" s="163" t="n"/>
       <c r="C54" s="86" t="n"/>
       <c r="D54" s="86" t="n"/>
       <c r="E54" s="86" t="n"/>
@@ -5511,7 +5754,7 @@
       <c r="A55" s="26" t="n">
         <v>33</v>
       </c>
-      <c r="B55" s="156" t="n"/>
+      <c r="B55" s="161" t="n"/>
       <c r="C55" s="86" t="n"/>
       <c r="D55" s="86" t="n"/>
       <c r="E55" s="86" t="n"/>
@@ -5591,7 +5834,7 @@
       <c r="A56" s="26" t="n">
         <v>34</v>
       </c>
-      <c r="B56" s="159" t="n"/>
+      <c r="B56" s="164" t="n"/>
       <c r="C56" s="86" t="n"/>
       <c r="D56" s="86" t="n"/>
       <c r="E56" s="86" t="n"/>
@@ -5671,7 +5914,7 @@
       <c r="A57" s="26" t="n">
         <v>35</v>
       </c>
-      <c r="B57" s="160" t="n"/>
+      <c r="B57" s="165" t="n"/>
       <c r="C57" s="86" t="n"/>
       <c r="D57" s="86" t="n"/>
       <c r="E57" s="86" t="n"/>
@@ -5751,7 +5994,7 @@
       <c r="A58" s="26" t="n">
         <v>36</v>
       </c>
-      <c r="B58" s="159" t="n"/>
+      <c r="B58" s="164" t="n"/>
       <c r="C58" s="86" t="n"/>
       <c r="D58" s="86" t="n"/>
       <c r="E58" s="86" t="n"/>
@@ -5831,7 +6074,7 @@
       <c r="A59" s="26" t="n">
         <v>37</v>
       </c>
-      <c r="B59" s="158" t="n"/>
+      <c r="B59" s="163" t="n"/>
       <c r="C59" s="86" t="n"/>
       <c r="D59" s="86" t="n"/>
       <c r="E59" s="86" t="n"/>
@@ -5911,7 +6154,7 @@
       <c r="A60" s="35" t="n">
         <v>38</v>
       </c>
-      <c r="B60" s="158" t="n"/>
+      <c r="B60" s="163" t="n"/>
       <c r="C60" s="86" t="n"/>
       <c r="D60" s="86" t="n"/>
       <c r="E60" s="86" t="n"/>
@@ -5991,7 +6234,7 @@
       <c r="A61" s="84" t="n">
         <v>39</v>
       </c>
-      <c r="B61" s="161" t="n"/>
+      <c r="B61" s="166" t="n"/>
       <c r="C61" s="86" t="n"/>
       <c r="D61" s="86" t="n"/>
       <c r="E61" s="86" t="n"/>
@@ -6071,7 +6314,7 @@
       <c r="A62" s="84" t="n">
         <v>40</v>
       </c>
-      <c r="B62" s="161" t="n"/>
+      <c r="B62" s="166" t="n"/>
       <c r="C62" s="86" t="n"/>
       <c r="D62" s="86" t="n"/>
       <c r="E62" s="86" t="n"/>
@@ -6151,7 +6394,7 @@
       <c r="A63" s="84" t="n">
         <v>41</v>
       </c>
-      <c r="B63" s="161" t="n"/>
+      <c r="B63" s="166" t="n"/>
       <c r="C63" s="86" t="n"/>
       <c r="D63" s="86" t="n"/>
       <c r="E63" s="86" t="n"/>
@@ -6231,7 +6474,7 @@
       <c r="A64" s="84" t="n">
         <v>42</v>
       </c>
-      <c r="B64" s="153" t="n"/>
+      <c r="B64" s="158" t="n"/>
       <c r="C64" s="86" t="n"/>
       <c r="D64" s="86" t="n"/>
       <c r="E64" s="86" t="n"/>
@@ -6311,7 +6554,7 @@
       <c r="A65" s="84" t="n">
         <v>43</v>
       </c>
-      <c r="B65" s="155" t="n"/>
+      <c r="B65" s="160" t="n"/>
       <c r="C65" s="86" t="n"/>
       <c r="D65" s="86" t="n"/>
       <c r="E65" s="86" t="n"/>
@@ -6391,7 +6634,7 @@
       <c r="A66" s="84" t="n">
         <v>44</v>
       </c>
-      <c r="B66" s="160" t="n"/>
+      <c r="B66" s="165" t="n"/>
       <c r="C66" s="86" t="n"/>
       <c r="D66" s="86" t="n"/>
       <c r="E66" s="86" t="n"/>
@@ -6471,7 +6714,7 @@
       <c r="A67" s="84" t="n">
         <v>45</v>
       </c>
-      <c r="B67" s="160" t="n"/>
+      <c r="B67" s="165" t="n"/>
       <c r="C67" s="86" t="n"/>
       <c r="D67" s="86" t="n"/>
       <c r="E67" s="86" t="n"/>
@@ -7499,7 +7742,7 @@
     <row r="1013" ht="15.75" customFormat="1" customHeight="1" s="1"/>
     <row r="1014" ht="15.75" customFormat="1" customHeight="1" s="1"/>
   </sheetData>
-  <mergeCells count="91">
+  <mergeCells count="101">
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="AL39:AP39"/>
     <mergeCell ref="AV39:AZ39"/>
@@ -7591,6 +7834,16 @@
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="M7:R7"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="M10:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>